<commit_message>
Added processes to the ReFramework and tested
</commit_message>
<xml_diff>
--- a/Database/Employee table template.xlsx
+++ b/Database/Employee table template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\premal\Google Drive\QAC projects\HR automation\Employee table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\premal\Google Drive\QAC projects\HR automation\automation\HR-Payroll-automation\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8DC4BC-F1CE-4802-9103-8D261CB62D4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC63B83E-39F1-4E7C-83AB-D5EF6BC747F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20880" yWindow="5340" windowWidth="16545" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,9 +419,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,7 +706,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,7 +714,7 @@
     <col min="8" max="8" width="9.140625" style="1"/>
     <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -753,7 +754,7 @@
       <c r="L1" t="s">
         <v>113</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>114</v>
       </c>
     </row>
@@ -781,7 +782,7 @@
       </c>
       <c r="H2" s="1">
         <f ca="1">RANDBETWEEN(7,25)</f>
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="I2">
         <v>80</v>
@@ -795,9 +796,9 @@
       <c r="L2">
         <v>0</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="2">
         <f ca="1">H2*I2</f>
-        <v>1280</v>
+        <v>560</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -824,7 +825,7 @@
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H21" ca="1" si="0">RANDBETWEEN(7,25)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I3">
         <v>80</v>
@@ -838,9 +839,9 @@
       <c r="L3">
         <v>0</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="2">
         <f t="shared" ref="M3:M21" ca="1" si="1">H3*I3</f>
-        <v>1040</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -867,7 +868,7 @@
       </c>
       <c r="H4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="I4">
         <v>80</v>
@@ -881,9 +882,9 @@
       <c r="L4">
         <v>0</v>
       </c>
-      <c r="M4" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>2000</v>
+      <c r="M4" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>640</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -910,7 +911,7 @@
       </c>
       <c r="H5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I5">
         <v>80</v>
@@ -924,9 +925,9 @@
       <c r="L5">
         <v>0</v>
       </c>
-      <c r="M5" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>560</v>
+      <c r="M5" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>640</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -953,7 +954,7 @@
       </c>
       <c r="H6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I6">
         <v>80</v>
@@ -967,9 +968,9 @@
       <c r="L6">
         <v>0</v>
       </c>
-      <c r="M6" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1440</v>
+      <c r="M6" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1680</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -996,7 +997,7 @@
       </c>
       <c r="H7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I7">
         <v>80</v>
@@ -1010,9 +1011,9 @@
       <c r="L7">
         <v>0</v>
       </c>
-      <c r="M7" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1520</v>
+      <c r="M7" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1600</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1039,7 +1040,7 @@
       </c>
       <c r="H8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I8">
         <v>80</v>
@@ -1053,9 +1054,9 @@
       <c r="L8">
         <v>0</v>
       </c>
-      <c r="M8" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1440</v>
+      <c r="M8" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>2000</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1082,7 +1083,7 @@
       </c>
       <c r="H9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="I9">
         <v>80</v>
@@ -1096,9 +1097,9 @@
       <c r="L9">
         <v>0</v>
       </c>
-      <c r="M9" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>720</v>
+      <c r="M9" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1840</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1125,7 +1126,7 @@
       </c>
       <c r="H10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I10">
         <v>80</v>
@@ -1139,9 +1140,9 @@
       <c r="L10">
         <v>0</v>
       </c>
-      <c r="M10" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1920</v>
+      <c r="M10" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1840</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1168,7 +1169,7 @@
       </c>
       <c r="H11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I11">
         <v>80</v>
@@ -1182,9 +1183,9 @@
       <c r="L11">
         <v>0</v>
       </c>
-      <c r="M11" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1200</v>
+      <c r="M11" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1120</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1211,7 +1212,7 @@
       </c>
       <c r="H12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I12">
         <v>80</v>
@@ -1225,9 +1226,9 @@
       <c r="L12">
         <v>0</v>
       </c>
-      <c r="M12" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1680</v>
+      <c r="M12" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1360</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1254,7 +1255,7 @@
       </c>
       <c r="H13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I13">
         <v>80</v>
@@ -1268,9 +1269,9 @@
       <c r="L13">
         <v>0</v>
       </c>
-      <c r="M13" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>560</v>
+      <c r="M13" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1040</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1297,7 +1298,7 @@
       </c>
       <c r="H14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="I14">
         <v>80</v>
@@ -1311,9 +1312,9 @@
       <c r="L14">
         <v>0</v>
       </c>
-      <c r="M14" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1920</v>
+      <c r="M14" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1440</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1340,7 +1341,7 @@
       </c>
       <c r="H15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="I15">
         <v>80</v>
@@ -1354,9 +1355,9 @@
       <c r="L15">
         <v>0</v>
       </c>
-      <c r="M15" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>720</v>
+      <c r="M15" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1120</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1383,7 +1384,7 @@
       </c>
       <c r="H16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I16">
         <v>80</v>
@@ -1397,9 +1398,9 @@
       <c r="L16">
         <v>0</v>
       </c>
-      <c r="M16" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>880</v>
+      <c r="M16" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>800</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1426,7 +1427,7 @@
       </c>
       <c r="H17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I17">
         <v>80</v>
@@ -1440,9 +1441,9 @@
       <c r="L17">
         <v>0</v>
       </c>
-      <c r="M17" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1120</v>
+      <c r="M17" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1040</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1469,7 +1470,7 @@
       </c>
       <c r="H18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I18">
         <v>80</v>
@@ -1483,9 +1484,9 @@
       <c r="L18">
         <v>0</v>
       </c>
-      <c r="M18" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1520</v>
+      <c r="M18" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1200</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1512,7 +1513,7 @@
       </c>
       <c r="H19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I19">
         <v>80</v>
@@ -1526,9 +1527,9 @@
       <c r="L19">
         <v>0</v>
       </c>
-      <c r="M19" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1200</v>
+      <c r="M19" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>880</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1555,7 +1556,7 @@
       </c>
       <c r="H20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I20">
         <v>80</v>
@@ -1569,9 +1570,9 @@
       <c r="L20">
         <v>0</v>
       </c>
-      <c r="M20" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1760</v>
+      <c r="M20" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1360</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1598,7 +1599,7 @@
       </c>
       <c r="H21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="I21">
         <v>80</v>
@@ -1612,9 +1613,9 @@
       <c r="L21">
         <v>0</v>
       </c>
-      <c r="M21" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1760</v>
+      <c r="M21" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>960</v>
       </c>
     </row>
   </sheetData>

</xml_diff>